<commit_message>
CIR model montecarlo working
</commit_message>
<xml_diff>
--- a/market_data/calculation_dividend_yield.xlsx
+++ b/market_data/calculation_dividend_yield.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\tfm_stochastic_dividends\market_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D80D28-0EA4-40BC-BFDC-820F5E54E7BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A3A30C-6FA2-4E11-A9D1-F010240D9795}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -176,12 +176,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -465,7 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19611,7 +19613,7 @@
         <v>3.968253968253968E-3</v>
       </c>
       <c r="F247">
-        <f>D247*252/(SUM(C247))</f>
+        <f t="shared" ref="F247:F252" si="165">D247*252/(SUM(C247))</f>
         <v>0.3067444097138744</v>
       </c>
       <c r="G247">
@@ -19691,7 +19693,7 @@
         <v>3.968253968253968E-3</v>
       </c>
       <c r="F248">
-        <f>D248*252/(SUM(C248))</f>
+        <f t="shared" si="165"/>
         <v>2.9019228043652898E-2</v>
       </c>
       <c r="G248">
@@ -19771,7 +19773,7 @@
         <v>3.968253968253968E-3</v>
       </c>
       <c r="F249">
-        <f>D249*252/(SUM(C249))</f>
+        <f t="shared" si="165"/>
         <v>0.15626707140979904</v>
       </c>
       <c r="G249">
@@ -19851,7 +19853,7 @@
         <v>3.968253968253968E-3</v>
       </c>
       <c r="F250">
-        <f>D250*252/(SUM(C250))</f>
+        <f t="shared" si="165"/>
         <v>0.59676299342983841</v>
       </c>
       <c r="G250">
@@ -19931,7 +19933,7 @@
         <v>3.968253968253968E-3</v>
       </c>
       <c r="F251">
-        <f>D251*252/(SUM(C251))</f>
+        <f t="shared" si="165"/>
         <v>0.11549374715381601</v>
       </c>
       <c r="G251">
@@ -20011,7 +20013,7 @@
         <v>3.968253968253968E-3</v>
       </c>
       <c r="F252">
-        <f>D252*252/(SUM(C252))</f>
+        <f t="shared" si="165"/>
         <v>0.28068726443627556</v>
       </c>
       <c r="G252">
@@ -20507,43 +20509,43 @@
         <v>3.8722602318816821</v>
       </c>
       <c r="K258">
-        <f t="shared" ref="K258:R258" si="165">IF(J258=0,J257,J258)</f>
+        <f t="shared" ref="K258:R258" si="166">IF(J258=0,J257,J258)</f>
         <v>3.8722602318816821</v>
       </c>
       <c r="L258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="M258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="N258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="O258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="P258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="Q258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="R258">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>3.8722602318816821</v>
       </c>
       <c r="S258">
-        <f t="shared" ref="S258:T258" si="166">IF(R258=0,R257,R258)</f>
+        <f t="shared" ref="S258:T258" si="167">IF(R258=0,R257,R258)</f>
         <v>3.8722602318816821</v>
       </c>
       <c r="T258">
-        <f t="shared" si="166"/>
+        <f t="shared" si="167"/>
         <v>3.8722602318816821</v>
       </c>
     </row>

</xml_diff>